<commit_message>
Completed another round of cross-matching
Added some more movies from Metacritic. Now will consolidate Bechdel test scores.
</commit_message>
<xml_diff>
--- a/data_2017_5_9/compare/nometa.xlsx
+++ b/data_2017_5_9/compare/nometa.xlsx
@@ -2139,7 +2139,7 @@
     <row r="61" spans="1:7" s="0" outlineLevel="0">
       <c r="A61" t="inlineStr">
         <is>
-          <t>anchorba10bab</t>
+          <t>anchorb10baby</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -7765,7 +7765,7 @@
     <row r="255" spans="1:7" s="0" outlineLevel="0">
       <c r="A255" t="inlineStr">
         <is>
-          <t>consumed15edi</t>
+          <t>consume15edii</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -10143,7 +10143,7 @@
     <row r="337" spans="1:7" s="0" outlineLevel="0">
       <c r="A337" t="inlineStr">
         <is>
-          <t>don’t'be10d</t>
+          <t>don'tbe10dark</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -11506,7 +11506,7 @@
     <row r="384" spans="1:7" s="0" outlineLevel="0">
       <c r="A384" t="inlineStr">
         <is>
-          <t>enkaerli01ori</t>
+          <t>enkaerl01orie</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -12724,7 +12724,7 @@
     <row r="426" spans="1:7" s="0" outlineLevel="0">
       <c r="A426" t="inlineStr">
         <is>
-          <t>forgivei06lin</t>
+          <t>forgive06lins</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -17973,7 +17973,7 @@
     <row r="607" spans="1:7" s="0" outlineLevel="0">
       <c r="A607" t="inlineStr">
         <is>
-          <t>islander06nde</t>
+          <t>islande06nder</t>
         </is>
       </c>
       <c r="B607" t="inlineStr">
@@ -29399,7 +29399,7 @@
     <row r="1001" spans="1:7" s="0" outlineLevel="0">
       <c r="A1001" t="inlineStr">
         <is>
-          <t>rakutent14dis</t>
+          <t>rakuten14dise</t>
         </is>
       </c>
       <c r="B1001" t="inlineStr">
@@ -33865,7 +33865,7 @@
     <row r="1155" spans="1:7" s="0" outlineLevel="0">
       <c r="A1155" t="inlineStr">
         <is>
-          <t>strength07nou</t>
+          <t>strengt07nour</t>
         </is>
       </c>
       <c r="B1155" t="inlineStr">
@@ -36591,7 +36591,7 @@
     <row r="1249" spans="1:7" s="0" outlineLevel="0">
       <c r="A1249" t="inlineStr">
         <is>
-          <t>waitingf07bli</t>
+          <t>waiting07blin</t>
         </is>
       </c>
       <c r="B1249" t="inlineStr">

</xml_diff>